<commit_message>
improve non-conformities and add threat assessment
</commit_message>
<xml_diff>
--- a/zorin_cybersecurity2/NonConformitiesPsono.xlsx
+++ b/zorin_cybersecurity2/NonConformitiesPsono.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Analysis" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -1664,7 +1664,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{002A00AB-003B-4E73-8AAE-00FA00A7001B}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00D2005B-0026-4773-ACE6-00FE0080002A}">
             <xm:f>"Yes"</xm:f>
             <x14:dxf>
               <font>
@@ -1681,7 +1681,7 @@
           <xm:sqref>C2:C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{0090002B-004D-4FCE-A670-006200D00024}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{006F000D-00E2-46EC-826B-0051002C0061}">
             <xm:f>"No"</xm:f>
             <x14:dxf>
               <font>
@@ -1698,7 +1698,7 @@
           <xm:sqref>C2:C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{004E000B-0087-429F-BC94-005400BD0060}">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00160071-00E7-4D99-967D-007400880016}">
             <xm:f>"Partial"</xm:f>
             <x14:dxf>
               <font>
@@ -1715,7 +1715,7 @@
           <xm:sqref>C2:C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{005F0078-004B-4C43-9A6C-0004006F0037}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{002000F8-00FC-4DF6-9F8A-00AF00FA0084}">
             <xm:f>"N/A"</xm:f>
             <x14:dxf>
               <border>

</xml_diff>